<commit_message>
New Experiment in generator ok
Se cambio la experimentacion del generador para hacer que genere casos con C-Estacionarios, M-Estacionarios y Fuertemente Estacionarios desde la funciomn solo diciendo que true a que quiere quesea asi la experimentacion
</commit_message>
<xml_diff>
--- a/experiment/linear/ex9.1.1/ex9.1.1(Linear).xlsx
+++ b/experiment/linear/ex9.1.1/ex9.1.1(Linear).xlsx
@@ -430,7 +430,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CAF0E20E-E4D8-9B45-9C94-E89B574F109C}">
-  <dimension ref="A1:L4"/>
+  <dimension ref="A1:L7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -588,6 +588,120 @@
         <v>1.9999999516271552</v>
       </c>
     </row>
+    <row r="5" spans="1:12">
+      <c r="A5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5">
+        <v>-13.0</v>
+      </c>
+      <c r="E5">
+        <v>0.001993264</v>
+      </c>
+      <c r="F5">
+        <v>0.01565619</v>
+      </c>
+      <c r="G5">
+        <v>0.0035683174604316543</v>
+      </c>
+      <c r="H5">
+        <v>2597</v>
+      </c>
+      <c r="I5">
+        <v>0.116912841796875</v>
+      </c>
+      <c r="J5">
+        <v>5.0</v>
+      </c>
+      <c r="K5">
+        <v>4.0</v>
+      </c>
+      <c r="L5">
+        <v>1.9999999999999996</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12">
+      <c r="A6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6">
+        <v>-13.0</v>
+      </c>
+      <c r="E6">
+        <v>0.004863592</v>
+      </c>
+      <c r="F6">
+        <v>0.02544338</v>
+      </c>
+      <c r="G6">
+        <v>0.009506216718095237</v>
+      </c>
+      <c r="H6">
+        <v>3079</v>
+      </c>
+      <c r="I6">
+        <v>0.1317291259765625</v>
+      </c>
+      <c r="J6">
+        <v>5.0</v>
+      </c>
+      <c r="K6">
+        <v>4.0</v>
+      </c>
+      <c r="L6">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12">
+      <c r="A7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D7">
+        <v>-13.000000246414976</v>
+      </c>
+      <c r="E7">
+        <v>0.01481231</v>
+      </c>
+      <c r="F7">
+        <v>0.032895627</v>
+      </c>
+      <c r="G7">
+        <v>0.020900470322175735</v>
+      </c>
+      <c r="H7">
+        <v>10616</v>
+      </c>
+      <c r="I7">
+        <v>0.29681396484375</v>
+      </c>
+      <c r="J7">
+        <v>5.000000032830815</v>
+      </c>
+      <c r="K7">
+        <v>4.000000038995717</v>
+      </c>
+      <c r="L7">
+        <v>1.9999999517014941</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>